<commit_message>
After Select List working
</commit_message>
<xml_diff>
--- a/retail system working.xlsx
+++ b/retail system working.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Screen</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>ADD-EDIT CUSTOMER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issues faced </t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,13 +476,13 @@
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="55" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="5" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -493,18 +496,21 @@
         <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -517,11 +523,12 @@
       <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -534,11 +541,12 @@
       <c r="E4" s="5">
         <v>42370</v>
       </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -548,11 +556,12 @@
       <c r="E5" s="5">
         <v>42370</v>
       </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -562,11 +571,12 @@
       <c r="E6" s="5">
         <v>42370</v>
       </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -576,11 +586,12 @@
       <c r="E7" s="5">
         <v>42371</v>
       </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -590,11 +601,12 @@
       <c r="E8" s="5">
         <v>42371</v>
       </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -604,11 +616,12 @@
       <c r="E9" s="5">
         <v>42372</v>
       </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -618,11 +631,12 @@
       <c r="E10" s="5">
         <v>42372</v>
       </c>
-      <c r="G10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -635,11 +649,12 @@
       <c r="E11" s="5">
         <v>42373</v>
       </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -649,11 +664,12 @@
       <c r="E12" s="5">
         <v>42373</v>
       </c>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -666,11 +682,12 @@
       <c r="E13" s="5">
         <v>42370</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" s="5"/>
+      <c r="H13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -680,11 +697,12 @@
       <c r="E14" s="5">
         <v>42371</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F14" s="5"/>
+      <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -694,11 +712,12 @@
       <c r="E15" s="5">
         <v>42372</v>
       </c>
-      <c r="G15" t="s">
+      <c r="F15" s="5"/>
+      <c r="H15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -708,40 +727,41 @@
       <c r="E16" s="5">
         <v>42372</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" s="5"/>
+      <c r="H16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
     </row>
   </sheetData>

</xml_diff>